<commit_message>
change the dashboard data from uploaded file xlsx
</commit_message>
<xml_diff>
--- a/storage/dataset.xlsx
+++ b/storage/dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kuliah\Semester 8\Skripsi\DATASET\skripsi-data-excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Braincore\Skripsi\comodity-price-predict\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246351A0-9EDA-4B19-AAD4-0B585A4D83E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61CB63C-1EFF-4BAC-B207-97F57B280CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{DEE3FCEA-EEAC-428E-AB03-5F42C9B4B7CE}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -100,7 +100,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B48D2AEB-64BC-4ACE-8A80-BC9CCE2014C3}">
   <dimension ref="A1:F1098"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1080" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
make a new blueprint for managing config file like upload xlsx, model, pkl file
</commit_message>
<xml_diff>
--- a/storage/dataset.xlsx
+++ b/storage/dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Braincore\Skripsi\comodity-price-predict\storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kuliah\Semester 8\Skripsi\DATASET\skripsi-data-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61CB63C-1EFF-4BAC-B207-97F57B280CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246351A0-9EDA-4B19-AAD4-0B585A4D83E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{DEE3FCEA-EEAC-428E-AB03-5F42C9B4B7CE}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -100,7 +100,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B48D2AEB-64BC-4ACE-8A80-BC9CCE2014C3}">
   <dimension ref="A1:F1098"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F14"/>
+    <sheetView tabSelected="1" topLeftCell="A1080" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>